<commit_message>
#bulkwhois Commit 22 May
</commit_message>
<xml_diff>
--- a/JavaBooks.xlsx
+++ b/JavaBooks.xlsx
@@ -12,11 +12,220 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>{
-   "ErrorMessage": {
-      "msg": "queries available for 103.251.221.74 is 0/20, please refill"
+   "WhoisRecord": {
+      "domainName": "savehindonriver.org",
+      "parseCode": 8,
+      "audit": {
+         "createdDate": "2018-05-21 05:36:42.000 UTC",
+         "updatedDate": "2018-05-21 05:36:42.000 UTC"
+      },
+      "registrarName": "GoDaddy.com, LLC",
+      "registrarIANAID": "146",
+      "registryData": {
+         "createdDate": "2017-09-13T16:02:51Z",
+         "updatedDate": "2017-11-13T03:46:55Z",
+         "expiresDate": "2018-09-13T16:02:51Z",
+         "registrant": {
+            "name": "Ashish sharma",
+            "organization": "Save Hindon River",
+            "street1": "Greater noida",
+            "city": "Noida",
+            "state": "Uttar Pradesh",
+            "postalCode": "201308",
+            "country": "INDIA",
+            "countryCode": "IN",
+            "email": "iashish.mariner@gmail.com",
+            "telephone": "919717373225",
+            "rawText": "Registrant Name: Ashish sharma\nRegistrant Organization: Save Hindon River\nRegistrant Street: Greater noida\nRegistrant City: Noida\nRegistrant State/Province: Uttar Pradesh\nRegistrant Postal Code: 201308\nRegistrant Country: IN\nRegistrant Phone: +91.9717373225\nRegistrant Email: iashish.mariner@gmail.com"
+         },
+         "administrativeContact": {
+            "name": "Ashish sharma",
+            "organization": "Save Hindon River",
+            "street1": "Greater noida",
+            "city": "Noida",
+            "state": "Uttar Pradesh",
+            "postalCode": "201308",
+            "country": "INDIA",
+            "countryCode": "IN",
+            "email": "iashish.mariner@gmail.com",
+            "telephone": "919717373225",
+            "rawText": "Admin Name: Ashish sharma\nAdmin Organization: Save Hindon River\nAdmin Street: Greater noida\nAdmin City: Noida\nAdmin State/Province: Uttar Pradesh\nAdmin Postal Code: 201308\nAdmin Country: IN\nAdmin Phone: +91.9717373225\nAdmin Email: iashish.mariner@gmail.com"
+         },
+         "technicalContact": {
+            "name": "Ashish sharma",
+            "organization": "Save Hindon River",
+            "street1": "Greater noida",
+            "city": "Noida",
+            "state": "Uttar Pradesh",
+            "postalCode": "201308",
+            "country": "INDIA",
+            "countryCode": "IN",
+            "email": "iashish.mariner@gmail.com",
+            "telephone": "919717373225",
+            "rawText": "Tech Name: Ashish sharma\nTech Organization: Save Hindon River\nTech Street: Greater noida\nTech City: Noida\nTech State/Province: Uttar Pradesh\nTech Postal Code: 201308\nTech Country: IN\nTech Phone: +91.9717373225\nTech Email: iashish.mariner@gmail.com"
+         },
+         "domainName": "savehindonriver.org",
+         "nameServers": {
+            "rawText": "NS75.DOMAINCONTROL.COM\nNS76.DOMAINCONTROL.COM\n",
+            "hostNames": [
+               "NS75.DOMAINCONTROL.COM",
+               "NS76.DOMAINCONTROL.COM"
+            ],
+            "ips": []
+         },
+         "status": "clientDeleteProhibited clientRenewProhibited clientTransferProhibited clientUpdateProhibited",
+         "rawText": "Domain Name: SAVEHINDONRIVER.ORG\nRegistry Domain ID: D402200000003589162-LROR\nRegistrar WHOIS Server: whois.godaddy.com\nRegistrar URL: http://www.godaddy.com\nUpdated Date: 2017-11-13T03:46:55Z\nCreation Date: 2017-09-13T16:02:51Z\nRegistry Expiry Date: 2018-09-13T16:02:51Z\nRegistrar Registration Expiration Date:\nRegistrar: GoDaddy.com, LLC\nRegistrar IANA ID: 146\nRegistrar Abuse Contact Email: abuse@godaddy.com\nRegistrar Abuse Contact Phone: +1.4806242505\nReseller:\nDomain Status: clientDeleteProhibited https://icann.org/epp#clientDeleteProhibited\nDomain Status: clientRenewProhibited https://icann.org/epp#clientRenewProhibited\nDomain Status: clientTransferProhibited https://icann.org/epp#clientTransferProhibited\nDomain Status: clientUpdateProhibited https://icann.org/epp#clientUpdateProhibited\nRegistry Registrant ID: C197004576-LROR\nRegistrant Name: Ashish sharma\nRegistrant Organization: Save Hindon River\nRegistrant Street: Greater noida\nRegistrant City: Noida\nRegistrant State/Province: Uttar Pradesh\nRegistrant Postal Code: 201308\nRegistrant Country: IN\nRegistrant Phone: +91.9717373225\nRegistrant Phone Ext:\nRegistrant Fax:\nRegistrant Fax Ext:\nRegistrant Email: iashish.mariner@gmail.com\nRegistry Admin ID: C197004578-LROR\nAdmin Name: Ashish sharma\nAdmin Organization: Save Hindon River\nAdmin Street: Greater noida\nAdmin City: Noida\nAdmin State/Province: Uttar Pradesh\nAdmin Postal Code: 201308\nAdmin Country: IN\nAdmin Phone: +91.9717373225\nAdmin Phone Ext:\nAdmin Fax:\nAdmin Fax Ext:\nAdmin Email: iashish.mariner@gmail.com\nRegistry Tech ID: C197004577-LROR\nTech Name: Ashish sharma\nTech Organization: Save Hindon River\nTech Street: Greater noida\nTech City: Noida\nTech State/Province: Uttar Pradesh\nTech Postal Code: 201308\nTech Country: IN\nTech Phone: +91.9717373225\nTech Phone Ext:\nTech Fax:\nTech Fax Ext:\nTech Email: iashish.mariner@gmail.com\nName Server: NS75.DOMAINCONTROL.COM\nName Server: NS76.DOMAINCONTROL.COM\nDNSSEC: unsigned\nURL of the ICANN Whois Inaccuracy Complaint Form: https://www.icann.org/wicf/\n&gt;&gt;&gt; Last update of WHOIS database: 2018-05-21T05:35:41Z &lt;&lt;&lt;\n\nFor more information on Whois status codes, please visit https://icann.org/epp\n\nAccess to Public Interest Registry WHOIS information is provided to assist persons in determining the contents of a domain name registration record in the Public Interest Registry registry database. The data in this record is provided by Public Interest Registry for informational purposes only, and Public Interest Registry does not guarantee its accuracy. This service is intended only for query-based access. You agree that you will use this data only for lawful purposes and that, under no circumstances will you use this data to: (a) allow, enable, or otherwise support the transmission by e-mail, telephone, or facsimile of mass unsolicited, commercial advertising or solicitations to entities other than the data recipient's own existing customers; or (b) enable high volume, automated, electronic processes that send queries or data to the systems of Registry Operator, a Registrar, or Afilias except as reasonably necessary to register domain names or modify existing registrations. All rights reserved. Public Interest Registry reserves the right to modify these terms at any time. By submitting this query, you agree to abide by this policy.",
+         "parseCode": 3579,
+         "header": "",
+         "strippedText": "Domain Name: SAVEHINDONRIVER.ORG\nRegistrar WHOIS Server: whois.godaddy.com\nRegistrar URL: http://www.godaddy.com\nUpdated Date: 2017-11-13T03:46:55Z\nCreation Date: 2017-09-13T16:02:51Z\nRegistry Expiry Date: 2018-09-13T16:02:51Z\nRegistrar: GoDaddy.com, LLC\nRegistrar IANA ID: 146\nRegistrar Abuse Contact Email: abuse@godaddy.com\nRegistrar Abuse Contact Phone: +1.4806242505\nDomain Status: clientDeleteProhibited https://icann.org/epp#clientDeleteProhibited\nDomain Status: clientRenewProhibited https://icann.org/epp#clientRenewProhibited\nDomain Status: clientTransferProhibited https://icann.org/epp#clientTransferProhibited\nDomain Status: clientUpdateProhibited https://icann.org/epp#clientUpdateProhibited\nRegistrant Name: Ashish sharma\nRegistrant Organization: Save Hindon River\nRegistrant Street: Greater noida\nRegistrant City: Noida\nRegistrant State/Province: Uttar Pradesh\nRegistrant Postal Code: 201308\nRegistrant Country: IN\nRegistrant Phone: +91.9717373225\nRegistrant Email: iashish.mariner@gmail.com\nAdmin Name: Ashish sharma\nAdmin Organization: Save Hindon River\nAdmin Street: Greater noida\nAdmin City: Noida\nAdmin State/Province: Uttar Pradesh\nAdmin Postal Code: 201308\nAdmin Country: IN\nAdmin Phone: +91.9717373225\nAdmin Email: iashish.mariner@gmail.com\nTech Name: Ashish sharma\nTech Organization: Save Hindon River\nTech Street: Greater noida\nTech City: Noida\nTech State/Province: Uttar Pradesh\nTech Postal Code: 201308\nTech Country: IN\nTech Phone: +91.9717373225\nTech Email: iashish.mariner@gmail.com\nName Server: NS75.DOMAINCONTROL.COM\nName Server: NS76.DOMAINCONTROL.COM\n",
+         "footer": "\n",
+         "audit": {
+            "createdDate": "2018-05-21 05:36:42.000 UTC",
+            "updatedDate": "2018-05-21 05:36:42.000 UTC"
+         },
+         "customField1Name": "RegistrarContactEmail",
+         "customField1Value": "abuse@godaddy.com",
+         "registrarName": "GoDaddy.com, LLC",
+         "registrarIANAID": "146",
+         "createdDateNormalized": "2017-09-13 16:02:51 UTC",
+         "updatedDateNormalized": "2017-11-13 03:46:55 UTC",
+         "expiresDateNormalized": "2018-09-13 16:02:51 UTC",
+         "customField2Name": "RegistrarContactPhone",
+         "customField3Name": "RegistrarURL",
+         "customField2Value": "+1.4806242505",
+         "customField3Value": "http://www.godaddy.com",
+         "whoisServer": "whois.godaddy.com"
+      },
+      "contactEmail": "iashish.mariner@gmail.com",
+      "domainNameExt": ".org",
+      "estimatedDomainAge": 249
+   }
+}</t>
+  </si>
+  <si>
+    <t>{
+   "WhoisRecord": {
+      "createdDate": "1992-11-04T05:00:00Z",
+      "updatedDate": "2018-03-03T01:23:13Z",
+      "expiresDate": "2018-11-03T04:00:00Z",
+      "registrant": {
+         "name": "Fresche Solutions Inc.",
+         "organization": "Fresche Solutions Inc.",
+         "street1": "995 Wellington",
+         "city": "Montreal",
+         "state": "QC",
+         "postalCode": "H3C1V3",
+         "country": "CANADA",
+         "countryCode": "CA",
+         "email": "andrew.bocchicchio@freschesolutions.com",
+         "telephone": "15147477007",
+         "fax": "15147473380",
+         "rawText": "Registrant Name: Fresche Solutions Inc.\nRegistrant Organization: Fresche Solutions Inc.\nRegistrant Street: 995 Wellington\nRegistrant City: Montreal\nRegistrant State/Province: QC\nRegistrant Postal Code: H3C1V3\nRegistrant Country: CA\nRegistrant Phone: +1.5147477007\nRegistrant Fax: +1.5147473380\nRegistrant Email: andrew.bocchicchio@freschesolutions.com"
+      },
+      "administrativeContact": {
+         "name": "Fresche Solutions Inc.",
+         "organization": "Fresche Solutions Inc.",
+         "street1": "995 Wellington",
+         "city": "Montreal",
+         "state": "QC",
+         "postalCode": "H3C1V3",
+         "country": "CANADA",
+         "countryCode": "CA",
+         "email": "andrew.bocchicchio@freschesolutions.com",
+         "telephone": "15147477007",
+         "fax": "15147473380",
+         "rawText": "Admin Name: Fresche Solutions Inc.\nAdmin Organization: Fresche Solutions Inc.\nAdmin Street: 995 Wellington\nAdmin City: Montreal\nAdmin State/Province: QC\nAdmin Postal Code: H3C1V3\nAdmin Country: CA\nAdmin Phone: +1.5147477007\nAdmin Fax: +1.5147473380\nAdmin Email: andrew.bocchicchio@freschesolutions.com"
+      },
+      "technicalContact": {
+         "name": "Bocchicchio, Andrew",
+         "organization": "Fresche Solutions Inc.",
+         "street1": "995 Wellington",
+         "city": "Montreal",
+         "state": "QC",
+         "postalCode": "H3C1V3",
+         "country": "CANADA",
+         "countryCode": "CA",
+         "email": "andrew.bocchicchio@freschelegacy.com",
+         "telephone": "5147477007",
+         "rawText": "Tech Name: Bocchicchio, Andrew\nTech Organization: Fresche Solutions Inc.\nTech Street: 995 Wellington\nTech City: Montreal\nTech State/Province: QC\nTech Postal Code: H3C1V3\nTech Country: CA\nTech Phone: 514-747-7007\nTech Email: andrew.bocchicchio@freschelegacy.com"
+      },
+      "domainName": "speedware.com",
+      "nameServers": {
+         "rawText": "CORE-WEB.SPEEDWARE.COM\nNS1.SPEEDWARE.COM\nMRH1.SPEEDWARE.COM\nNS1.TWISTED4LIFE.COM\n",
+         "hostNames": [
+            "CORE-WEB.SPEEDWARE.COM",
+            "NS1.SPEEDWARE.COM",
+            "MRH1.SPEEDWARE.COM",
+            "NS1.TWISTED4LIFE.COM"
+         ],
+         "ips": []
+      },
+      "status": "clientTransferProhibited",
+      "rawText": "Domain Name: SPEEDWARE.COM\nRegistry Domain ID: 2775194_DOMAIN_COM-VRSN\nRegistrar WHOIS Server: whois.networksolutions.com\nRegistrar URL: http://networksolutions.com\nUpdated Date: 2018-03-03T01:23:13Z\nCreation Date: 1992-11-04T05:00:00Z\nRegistrar Registration Expiration Date: 2018-11-03T04:00:00Z\nRegistrar: NETWORK SOLUTIONS, LLC.\nRegistrar IANA ID: 2\nReseller: \nDomain Status: clientTransferProhibited https://icann.org/epp#clientTransferProhibited\nRegistry Registrant ID: \nRegistrant Name: Fresche Solutions Inc.\nRegistrant Organization: Fresche Solutions Inc.\nRegistrant Street: 995 Wellington\nRegistrant City: Montreal\nRegistrant State/Province: QC\nRegistrant Postal Code: H3C1V3\nRegistrant Country: CA\nRegistrant Phone: +1.5147477007\nRegistrant Phone Ext: \nRegistrant Fax: +1.5147473380\nRegistrant Fax Ext: \nRegistrant Email: andrew.bocchicchio@freschesolutions.com\nRegistry Admin ID: \nAdmin Name: Fresche Solutions Inc.\nAdmin Organization: Fresche Solutions Inc.\nAdmin Street: 995 Wellington\nAdmin City: Montreal\nAdmin State/Province: QC\nAdmin Postal Code: H3C1V3\nAdmin Country: CA\nAdmin Phone: +1.5147477007\nAdmin Phone Ext: \nAdmin Fax: +1.5147473380\nAdmin Fax Ext: \nAdmin Email: andrew.bocchicchio@freschesolutions.com\nRegistry Tech ID: \nTech Name: Bocchicchio, Andrew\nTech Organization: Fresche Solutions Inc.\nTech Street: 995 Wellington\nTech City: Montreal\nTech State/Province: QC\nTech Postal Code: H3C1V3\nTech Country: CA\nTech Phone: 514-747-7007\nTech Phone Ext: \nTech Fax: \nTech Fax Ext: \nTech Email: andrew.bocchicchio@freschelegacy.com\nName Server: CORE-WEB.SPEEDWARE.COM\nName Server: NS1.SPEEDWARE.COM\nName Server: MRH1.SPEEDWARE.COM\nName Server: NS1.TWISTED4LIFE.COM\nDNSSEC: unsigned\nRegistrar Abuse Contact Email: abuse@web.com\nRegistrar Abuse Contact Phone: +1.8003337680\nURL of the ICANN WHOIS Data Problem Reporting System: http://wdprs.internic.net/\n&gt;&gt;&gt; Last update of WHOIS database: 2018-05-21T05:36:21Z &lt;&lt;&lt;\n\nFor more information on Whois status codes, please visit https://www.icann.org/resources/pages/epp-status-codes-2014-06-16-en\n\n\nThe data in Networksolutions.com's WHOIS database is provided to you by\nNetworksolutions.com for information purposes only, that is, to assist you in\nobtaining information about or related to a domain name registration\nrecord. Networksolutions.com makes this information available \"as is,\" and\ndoes not guarantee its accuracy. By submitting a WHOIS query, you\nagree that you will use this data only for lawful purposes and that,\nunder no circumstances will you use this data to: (1) allow, enable,\nor otherwise support the transmission of mass unsolicited, commercial\nadvertising or solicitations via direct mail, electronic mail, or by\ntelephone; or (2) enable high volume, automated, electronic processes\nthat apply to Networksolutions.com  (or its systems). The compilation,\nrepackaging, dissemination or other use of this data is expressly\nprohibited without the prior written consent of Networksolutions.com.\nNetworksolutions.com reserves the right to modify these terms at any time.\nBy submitting this query, you agree to abide by these terms.\n\nFor more information on Whois status codes, please visit\nhttps://www.icann.org/resources/pages/epp-status-codes-2014-06-16-en.",
+      "parseCode": 3579,
+      "header": "",
+      "strippedText": "Domain Name: SPEEDWARE.COM\nRegistrar WHOIS Server: whois.networksolutions.com\nRegistrar URL: http://networksolutions.com\nUpdated Date: 2018-03-03T01:23:13Z\nCreation Date: 1992-11-04T05:00:00Z\nRegistrar Registration Expiration Date: 2018-11-03T04:00:00Z\nRegistrar: NETWORK SOLUTIONS, LLC.\nRegistrar IANA ID: 2\nDomain Status: clientTransferProhibited https://icann.org/epp#clientTransferProhibited\nRegistrant Name: Fresche Solutions Inc.\nRegistrant Organization: Fresche Solutions Inc.\nRegistrant Street: 995 Wellington\nRegistrant City: Montreal\nRegistrant State/Province: QC\nRegistrant Postal Code: H3C1V3\nRegistrant Country: CA\nRegistrant Phone: +1.5147477007\nRegistrant Fax: +1.5147473380\nRegistrant Email: andrew.bocchicchio@freschesolutions.com\nAdmin Name: Fresche Solutions Inc.\nAdmin Organization: Fresche Solutions Inc.\nAdmin Street: 995 Wellington\nAdmin City: Montreal\nAdmin State/Province: QC\nAdmin Postal Code: H3C1V3\nAdmin Country: CA\nAdmin Phone: +1.5147477007\nAdmin Fax: +1.5147473380\nAdmin Email: andrew.bocchicchio@freschesolutions.com\nTech Name: Bocchicchio, Andrew\nTech Organization: Fresche Solutions Inc.\nTech Street: 995 Wellington\nTech City: Montreal\nTech State/Province: QC\nTech Postal Code: H3C1V3\nTech Country: CA\nTech Phone: 514-747-7007\nTech Email: andrew.bocchicchio@freschelegacy.com\nName Server: CORE-WEB.SPEEDWARE.COM\nName Server: NS1.SPEEDWARE.COM\nName Server: MRH1.SPEEDWARE.COM\nName Server: NS1.TWISTED4LIFE.COM\nRegistrar Abuse Contact Email: abuse@web.com\nRegistrar Abuse Contact Phone: +1.8003337680\n",
+      "footer": "\n",
+      "audit": {
+         "createdDate": "2018-05-21 05:36:51.000 UTC",
+         "updatedDate": "2018-05-21 05:36:51.000 UTC"
+      },
+      "customField1Name": "RegistrarContactEmail",
+      "customField1Value": "abuse@web.com",
+      "registrarName": "NETWORK SOLUTIONS, LLC.",
+      "registrarIANAID": "2",
+      "whoisServer": "whois.networksolutions.com",
+      "createdDateNormalized": "1992-11-04 05:00:00 UTC",
+      "updatedDateNormalized": "2018-03-03 01:23:13 UTC",
+      "expiresDateNormalized": "2018-11-03 04:00:00 UTC",
+      "customField2Name": "RegistrarContactPhone",
+      "customField3Name": "RegistrarURL",
+      "customField2Value": "+1.8003337680",
+      "customField3Value": "http://networksolutions.com",
+      "registryData": {
+         "createdDate": "1992-11-04T05:00:00Z",
+         "updatedDate": "2017-01-30T13:58:31Z",
+         "expiresDate": "2018-11-03T04:00:00Z",
+         "domainName": "speedware.com",
+         "nameServers": {
+            "rawText": "CORE-WEB.SPEEDWARE.COM\nMRH1.SPEEDWARE.COM\nNS1.SPEEDWARE.COM\nNS1.TWISTED4LIFE.COM\n",
+            "hostNames": [
+               "CORE-WEB.SPEEDWARE.COM",
+               "MRH1.SPEEDWARE.COM",
+               "NS1.SPEEDWARE.COM",
+               "NS1.TWISTED4LIFE.COM"
+            ],
+            "ips": []
+         },
+         "status": "clientTransferProhibited",
+         "rawText": "Domain Name: SPEEDWARE.COM\n   Registry Domain ID: 2775194_DOMAIN_COM-VRSN\n   Registrar WHOIS Server: whois.networksolutions.com\n   Registrar URL: http://networksolutions.com\n   Updated Date: 2017-01-30T13:58:31Z\n   Creation Date: 1992-11-04T05:00:00Z\n   Registry Expiry Date: 2018-11-03T04:00:00Z\n   Registrar: Network Solutions, LLC.\n   Registrar IANA ID: 2\n   Registrar Abuse Contact Email: abuse@web.com\n   Registrar Abuse Contact Phone: +1.8003337680\n   Domain Status: clientTransferProhibited https://icann.org/epp#clientTransferProhibited\n   Name Server: CORE-WEB.SPEEDWARE.COM\n   Name Server: MRH1.SPEEDWARE.COM\n   Name Server: NS1.SPEEDWARE.COM\n   Name Server: NS1.TWISTED4LIFE.COM\n   DNSSEC: unsigned\n   URL of the ICANN Whois Inaccuracy Complaint Form: https://www.icann.org/wicf/\n&gt;&gt;&gt; Last update of whois database: 2018-05-21T05:36:39Z &lt;&lt;&lt;\n\nFor more information on Whois status codes, please visit https://icann.org/epp\n\nNOTICE: The expiration date displayed in this record is the date the\nregistrar's sponsorship of the domain name registration in the registry is\ncurrently set to expire. This date does not necessarily reflect the expiration\ndate of the domain name registrant's agreement with the sponsoring\nregistrar.  Users may consult the sponsoring registrar's Whois database to\nview the registrar's reported date of expiration for this registration.\n\nTERMS OF USE: You are not authorized to access or query our Whois\ndatabase through the use of electronic processes that are high-volume and\nautomated except as reasonably necessary to register domain names or\nmodify existing registrations; the Data in VeriSign Global Registry\nServices' (\"VeriSign\") Whois database is provided by VeriSign for\ninformation purposes only, and to assist persons in obtaining information\nabout or related to a domain name registration record. VeriSign does not\nguarantee its accuracy. By submitting a Whois query, you agree to abide\nby the following terms of use: You agree that you may use this Data only\nfor lawful purposes and that under no circumstances will you use this Data\nto: (1) allow, enable, or otherwise support the transmission of mass\nunsolicited, commercial advertising or solicitations via e-mail, telephone,\nor facsimile; or (2) enable high volume, automated, electronic processes\nthat apply to VeriSign (or its computer systems). The compilation,\nrepackaging, dissemination or other use of this Data is expressly\nprohibited without the prior written consent of VeriSign. You agree not to\nuse electronic processes that are automated and high-volume to access or\nquery the Whois database except as reasonably necessary to register\ndomain names or modify existing registrations. VeriSign reserves the right\nto restrict your access to the Whois database in its sole discretion to ensure\noperational stability.  VeriSign may restrict or terminate your access to the\nWhois database for failure to abide by these terms of use. VeriSign\nreserves the right to modify these terms at any time.\n\nThe Registry database contains ONLY .COM, .NET, .EDU domains and\nRegistrars.",
+         "parseCode": 251,
+         "header": "",
+         "strippedText": "Domain Name: SPEEDWARE.COM\nRegistry Domain ID: 2775194_DOMAIN_COM-VRSN\nRegistrar WHOIS Server: whois.networksolutions.com\nRegistrar URL: http://networksolutions.com\nUpdated Date: 2017-01-30T13:58:31Z\nCreation Date: 1992-11-04T05:00:00Z\nRegistry Expiry Date: 2018-11-03T04:00:00Z\nRegistrar: Network Solutions, LLC.\nRegistrar IANA ID: 2\nRegistrar Abuse Contact Email: abuse@web.com\nRegistrar Abuse Contact Phone: +1.8003337680\nDomain Status: clientTransferProhibited https://icann.org/epp#clientTransferProhibited\nName Server: CORE-WEB.SPEEDWARE.COM\nName Server: MRH1.SPEEDWARE.COM\nName Server: NS1.SPEEDWARE.COM\nName Server: NS1.TWISTED4LIFE.COM\nDNSSEC: unsigned\nURL of the ICANN Whois Inaccuracy Complaint Form: https://www.icann.org/wicf/\n&gt;&gt;&gt; Last update of whois database: 2018-05-21T05:36:39Z &lt;&lt;&lt;\nFor more information on Whois status codes, please visit https://icann.org/epp\nNOTICE: The expiration date displayed in this record is the date the\nregistrar's sponsorship of the domain name registration in the registry is\ncurrently set to expire. This date does not necessarily reflect the expiration\ndate of the domain name registrant's agreement with the sponsoring\nregistrar.  Users may consult the sponsoring registrar's Whois database to\nview the registrar's reported date of expiration for this registration.\nTERMS OF USE: You are not authorized to access or query our Whois\ndatabase through the use of electronic processes that are high-volume and\nautomated except as reasonably necessary to register domain names or\nmodify existing registrations; the Data in VeriSign Global Registry\nServices' (\"VeriSign\") Whois database is provided by VeriSign for\ninformation purposes only, and to assist persons in obtaining information\nabout or related to a domain name registration record. VeriSign does not\nguarantee its accuracy. By submitting a Whois query, you agree to abide\nby the following terms of use: You agree that you may use this Data only\nfor lawful purposes and that under no circumstances will you use this Data\nto: (1) allow, enable, or otherwise support the transmission of mass\nunsolicited, commercial advertising or solicitations via e-mail, telephone,\nor facsimile; or (2) enable high volume, automated, electronic processes\nthat apply to VeriSign (or its computer systems). The compilation,\nrepackaging, dissemination or other use of this Data is expressly\nprohibited without the prior written consent of VeriSign. You agree not to\nuse electronic processes that are automated and high-volume to access or\nquery the Whois database except as reasonably necessary to register\ndomain names or modify existing registrations. VeriSign reserves the right\nto restrict your access to the Whois database in its sole discretion to ensure\noperational stability.  VeriSign may restrict or terminate your access to the\nWhois database for failure to abide by these terms of use. VeriSign\nreserves the right to modify these terms at any time.\nThe Registry database contains ONLY .COM, .NET, .EDU domains and\nRegistrars.\n",
+         "footer": "\n",
+         "audit": {
+            "createdDate": "2018-05-21 05:36:49.000 UTC",
+            "updatedDate": "2018-05-21 05:36:49.000 UTC"
+         },
+         "customField1Name": "RegistrarContactEmail",
+         "customField1Value": "abuse@web.com",
+         "registrarName": "Network Solutions, LLC.",
+         "registrarIANAID": "2",
+         "createdDateNormalized": "1992-11-04 05:00:00 UTC",
+         "updatedDateNormalized": "2017-01-30 13:58:31 UTC",
+         "expiresDateNormalized": "2018-11-03 04:00:00 UTC",
+         "customField2Name": "RegistrarContactPhone",
+         "customField3Name": "RegistrarURL",
+         "customField2Value": "+1.8003337680",
+         "customField3Value": "http://networksolutions.com",
+         "whoisServer": "whois.networksolutions.com"
+      },
+      "contactEmail": "andrew.bocchicchio@freschesolutions.com",
+      "domainNameExt": ".com",
+      "estimatedDomainAge": 9329
    }
 }</t>
   </si>
@@ -76,7 +285,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>